<commit_message>
Criação dos exercícios extras e atualização das presenças
</commit_message>
<xml_diff>
--- a/organizacao/presencas.xlsx
+++ b/organizacao/presencas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\senai-dev-2s2019\organizacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE5F462-31DD-41F6-9ACE-CB81D5FE6851}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7AE3A6-AAFD-4CA3-B070-2E712FC4A17A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="84">
   <si>
     <t>NOME</t>
   </si>
@@ -966,11 +966,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DA29"/>
+  <dimension ref="A1:DA40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z13" sqref="Z13"/>
+      <selection pane="topRight" activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1789,12 +1789,12 @@
       <c r="P10" s="14">
         <v>5</v>
       </c>
-      <c r="Q10" s="14" t="s">
-        <v>82</v>
+      <c r="Q10" s="14">
+        <v>3</v>
       </c>
       <c r="DA10" s="1">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:105" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -3003,6 +3003,9 @@
     </row>
     <row r="29" spans="1:105" x14ac:dyDescent="0.25">
       <c r="U29" s="37"/>
+    </row>
+    <row r="40" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R40" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>